<commit_message>
bug with surv. data fixed
</commit_message>
<xml_diff>
--- a/dat/surveillance_data.xlsx
+++ b/dat/surveillance_data.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="287">
   <si>
     <t>paragraph</t>
   </si>
@@ -714,13 +714,13 @@
     <t>Neue psychoaktive Substanzen (§ 100a Abs. 2 Nr. 9a StPO)</t>
   </si>
   <si>
-    <t>Erstanordnungen 1.777</t>
+    <t xml:space="preserve">Erstanordnungen </t>
   </si>
   <si>
     <t>Festnetztelekommunikation</t>
   </si>
   <si>
-    <t>Mobilfunktelekommunikation 1.920</t>
+    <t>Mobilfunktelekommunikation</t>
   </si>
   <si>
     <t>5.3</t>
@@ -847,9 +847,6 @@
   </si>
   <si>
     <t>Straftaten nach § 52 Abs. 1 Nr. 1 und 2Buchstabe c und d sowie Abs. 5 und 6 Waffengesetz (§ 100a Abs. 2 Nr. 11b StPO)</t>
-  </si>
-  <si>
-    <t>Mobilfunktelekommunikation</t>
   </si>
   <si>
     <t>Straftaten des Friedensverrats, des Hochverratsund der Gefährdung des demokratischenRechtsstaates sowie des Landesverrats und derGefährdung der äußeren Sicherheit (§ 100a Abs. 2 Nr. 1a StPO)</t>
@@ -1188,8 +1185,22 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="8.63"/>
+    <col customWidth="1" min="2" max="2" width="11.25"/>
     <col customWidth="1" min="3" max="3" width="29.38"/>
-    <col customWidth="1" min="4" max="4" width="49.88"/>
+    <col customWidth="1" min="4" max="4" width="27.88"/>
+    <col customWidth="1" min="5" max="7" width="4.75"/>
+    <col customWidth="1" min="8" max="8" width="3.75"/>
+    <col customWidth="1" min="9" max="9" width="3.63"/>
+    <col customWidth="1" min="10" max="10" width="3.75"/>
+    <col customWidth="1" min="11" max="11" width="4.75"/>
+    <col customWidth="1" min="12" max="12" width="3.75"/>
+    <col customWidth="1" min="13" max="13" width="4.75"/>
+    <col customWidth="1" min="14" max="15" width="3.75"/>
+    <col customWidth="1" min="16" max="16" width="3.0"/>
+    <col customWidth="1" min="17" max="20" width="3.75"/>
+    <col customWidth="1" min="21" max="21" width="4.5"/>
+    <col customWidth="1" min="22" max="22" width="5.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -9355,7 +9366,19 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="8.63"/>
+    <col customWidth="1" min="2" max="2" width="11.25"/>
     <col customWidth="1" min="3" max="3" width="20.5"/>
+    <col customWidth="1" min="4" max="6" width="4.75"/>
+    <col customWidth="1" min="7" max="9" width="3.75"/>
+    <col customWidth="1" min="10" max="10" width="4.75"/>
+    <col customWidth="1" min="11" max="11" width="3.75"/>
+    <col customWidth="1" min="12" max="12" width="4.75"/>
+    <col customWidth="1" min="13" max="14" width="3.75"/>
+    <col customWidth="1" min="15" max="15" width="3.0"/>
+    <col customWidth="1" min="16" max="19" width="3.75"/>
+    <col customWidth="1" min="20" max="20" width="4.5"/>
+    <col customWidth="1" min="21" max="21" width="5.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -15413,6 +15436,20 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="8.63"/>
+    <col customWidth="1" min="2" max="2" width="11.25"/>
+    <col customWidth="1" min="4" max="6" width="4.75"/>
+    <col customWidth="1" min="7" max="9" width="3.75"/>
+    <col customWidth="1" min="10" max="10" width="4.75"/>
+    <col customWidth="1" min="11" max="11" width="3.75"/>
+    <col customWidth="1" min="12" max="12" width="4.75"/>
+    <col customWidth="1" min="13" max="14" width="3.75"/>
+    <col customWidth="1" min="15" max="15" width="3.0"/>
+    <col customWidth="1" min="16" max="19" width="3.75"/>
+    <col customWidth="1" min="20" max="20" width="4.5"/>
+    <col customWidth="1" min="21" max="21" width="5.88"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -23310,7 +23347,16 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
+    <col customWidth="1" min="1" max="1" width="8.63"/>
+    <col customWidth="1" min="2" max="2" width="11.25"/>
     <col customWidth="1" min="3" max="3" width="34.75"/>
+    <col customWidth="1" min="4" max="4" width="4.75"/>
+    <col customWidth="1" min="5" max="5" width="5.13"/>
+    <col customWidth="1" min="6" max="7" width="3.75"/>
+    <col customWidth="1" min="8" max="12" width="4.75"/>
+    <col customWidth="1" min="13" max="19" width="3.75"/>
+    <col customWidth="1" min="20" max="20" width="4.5"/>
+    <col customWidth="1" min="21" max="21" width="5.88"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -23454,43 +23500,43 @@
         <v>227</v>
       </c>
       <c r="D3" s="1">
+        <v>1777.0</v>
+      </c>
+      <c r="E3" s="1">
         <v>3512.0</v>
       </c>
-      <c r="E3" s="1">
+      <c r="F3" s="1">
         <v>1503.0</v>
       </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>222.0</v>
       </c>
-      <c r="G3" s="1">
+      <c r="H3" s="1">
         <v>235.0</v>
       </c>
-      <c r="H3" s="1">
+      <c r="I3" s="1">
         <v>1028.0</v>
       </c>
-      <c r="I3" s="1">
+      <c r="J3" s="1">
         <v>2728.0</v>
       </c>
-      <c r="J3" s="1">
+      <c r="K3" s="1">
         <v>281.0</v>
       </c>
-      <c r="K3" s="1">
+      <c r="L3" s="1">
         <v>1646.0</v>
       </c>
-      <c r="L3" s="1">
+      <c r="M3" s="1">
         <v>1549.0</v>
       </c>
-      <c r="M3" s="1">
+      <c r="N3" s="1">
         <v>555.0</v>
       </c>
-      <c r="N3" s="1">
+      <c r="O3" s="1">
         <v>209.0</v>
       </c>
-      <c r="O3" s="1">
-        <v>8.0</v>
-      </c>
       <c r="P3" s="1">
-        <v>18.0</v>
+        <v>818.0</v>
       </c>
       <c r="Q3" s="1">
         <v>346.0</v>
@@ -23649,43 +23695,43 @@
         <v>229</v>
       </c>
       <c r="D6" s="1">
+        <v>1920.0</v>
+      </c>
+      <c r="E6" s="1">
         <v>3542.0</v>
       </c>
-      <c r="E6" s="1">
+      <c r="F6" s="1">
         <v>1692.0</v>
       </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>565.0</v>
       </c>
-      <c r="G6" s="1">
+      <c r="H6" s="1">
         <v>302.0</v>
       </c>
-      <c r="H6" s="1">
+      <c r="I6" s="1">
         <v>1155.0</v>
       </c>
-      <c r="I6" s="1">
+      <c r="J6" s="1">
         <v>5094.0</v>
       </c>
-      <c r="J6" s="1">
+      <c r="K6" s="1">
         <v>275.0</v>
       </c>
-      <c r="K6" s="1">
+      <c r="L6" s="1">
         <v>1710.0</v>
       </c>
-      <c r="L6" s="1">
+      <c r="M6" s="1">
         <v>1533.0</v>
       </c>
-      <c r="M6" s="1">
+      <c r="N6" s="1">
         <v>713.0</v>
       </c>
-      <c r="N6" s="1">
+      <c r="O6" s="1">
         <v>235.0</v>
       </c>
-      <c r="O6" s="1">
-        <v>9.0</v>
-      </c>
       <c r="P6" s="1">
-        <v>61.0</v>
+        <v>961.0</v>
       </c>
       <c r="Q6" s="1">
         <v>425.0</v>
@@ -30198,6 +30244,22 @@
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <cols>
+    <col customWidth="1" min="1" max="1" width="8.63"/>
+    <col customWidth="1" min="2" max="2" width="11.25"/>
+    <col customWidth="1" min="4" max="4" width="4.75"/>
+    <col customWidth="1" min="5" max="5" width="5.13"/>
+    <col customWidth="1" min="6" max="6" width="4.75"/>
+    <col customWidth="1" min="7" max="8" width="3.75"/>
+    <col customWidth="1" min="9" max="10" width="4.75"/>
+    <col customWidth="1" min="11" max="11" width="3.75"/>
+    <col customWidth="1" min="12" max="13" width="4.75"/>
+    <col customWidth="1" min="14" max="15" width="3.75"/>
+    <col customWidth="1" min="16" max="16" width="4.75"/>
+    <col customWidth="1" min="17" max="19" width="3.75"/>
+    <col customWidth="1" min="20" max="20" width="4.5"/>
+    <col customWidth="1" min="21" max="21" width="5.88"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
@@ -30532,7 +30594,7 @@
         <v>34</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>272</v>
+        <v>229</v>
       </c>
       <c r="D6" s="1">
         <v>2000.0</v>
@@ -30662,7 +30724,7 @@
         <v>37</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="D8" s="1">
         <v>9.0</v>
@@ -30727,7 +30789,7 @@
         <v>40</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="D9" s="1">
         <v>0.0</v>
@@ -31052,7 +31114,7 @@
         <v>55</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D14" s="1">
         <v>4.0</v>
@@ -32027,7 +32089,7 @@
         <v>106</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D29" s="1">
         <v>40.0</v>
@@ -32157,7 +32219,7 @@
         <v>112</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D31" s="1">
         <v>39.0</v>
@@ -32222,7 +32284,7 @@
         <v>115</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="D32" s="1">
         <v>0.0</v>
@@ -32287,7 +32349,7 @@
         <v>118</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="D33" s="1">
         <v>0.0</v>
@@ -32482,7 +32544,7 @@
         <v>130</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="D36" s="1">
         <v>6.0</v>
@@ -32547,7 +32609,7 @@
         <v>133</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="D37" s="1">
         <v>221.0</v>
@@ -32612,7 +32674,7 @@
         <v>136</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D38" s="1">
         <v>947.0</v>
@@ -32677,7 +32739,7 @@
         <v>139</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D39" s="1">
         <v>0.0</v>
@@ -32742,7 +32804,7 @@
         <v>142</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="D40" s="1">
         <v>4.0</v>
@@ -32807,7 +32869,7 @@
         <v>144</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D41" s="1">
         <v>4.0</v>
@@ -33067,7 +33129,7 @@
         <v>162</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D45" s="1">
         <v>12.0</v>
@@ -33132,7 +33194,7 @@
         <v>165</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D46" s="1">
         <v>18.0</v>

</xml_diff>

<commit_message>
added mobile user data & additional surveillance years
</commit_message>
<xml_diff>
--- a/dat/surveillance_data.xlsx
+++ b/dat/surveillance_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jakob/Code_Uni/DataLiteracy/dat/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C67F7FA2-3225-B549-9363-A923FBEE35EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0E3A110-AD3F-3D44-AC8F-A4A24B0BCCE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19380" yWindow="-920" windowWidth="19000" windowHeight="21100" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-40" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021_surveillance" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,10 @@
     <sheet name="2014_surveillance" sheetId="11" r:id="rId8"/>
     <sheet name="2013_surveillance" sheetId="7" r:id="rId9"/>
     <sheet name="2012_surveillance" sheetId="8" r:id="rId10"/>
-    <sheet name="2010_surveillance" sheetId="9" r:id="rId11"/>
+    <sheet name="2011_surveillance" sheetId="14" r:id="rId11"/>
+    <sheet name="2010_surveillance" sheetId="9" r:id="rId12"/>
+    <sheet name="2009_surveillance" sheetId="13" r:id="rId13"/>
+    <sheet name="2008_surveillance" sheetId="12" r:id="rId14"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -55,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="289">
   <si>
     <t>paragraph</t>
   </si>
@@ -920,12 +923,15 @@
   <si>
     <t>Straftaten nach § 52 Abs. 1 Nr. 1, 2 Buchstabe cund d sowie Abs. 5 und 6 Waffengesetz (§ 100aAbs. 2 Nr. 11b StPO)</t>
   </si>
+  <si>
+    <t>162</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -948,6 +954,12 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -979,7 +991,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -987,6 +999,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1207,7 +1220,7 @@
   </sheetPr>
   <dimension ref="A1:V1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9389,7 +9402,9 @@
   </sheetPr>
   <dimension ref="A1:U958"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M17" sqref="M17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -9398,10 +9413,12 @@
     <col min="4" max="4" width="4.6640625" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" customWidth="1"/>
     <col min="6" max="6" width="4.6640625" customWidth="1"/>
-    <col min="7" max="8" width="3.6640625" customWidth="1"/>
+    <col min="7" max="7" width="6.5" customWidth="1"/>
+    <col min="8" max="8" width="3.6640625" customWidth="1"/>
     <col min="9" max="10" width="4.6640625" customWidth="1"/>
     <col min="11" max="11" width="3.6640625" customWidth="1"/>
-    <col min="12" max="13" width="4.6640625" customWidth="1"/>
+    <col min="12" max="12" width="4.6640625" customWidth="1"/>
+    <col min="13" max="13" width="8.33203125" customWidth="1"/>
     <col min="14" max="15" width="3.6640625" customWidth="1"/>
     <col min="16" max="16" width="4.6640625" customWidth="1"/>
     <col min="17" max="19" width="3.6640625" customWidth="1"/>
@@ -9484,59 +9501,59 @@
       <c r="C2" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D2" s="1">
-        <v>2062</v>
-      </c>
-      <c r="E2" s="1">
-        <v>6348</v>
-      </c>
-      <c r="F2" s="1">
-        <v>433</v>
-      </c>
-      <c r="G2" s="1">
-        <v>191</v>
-      </c>
-      <c r="H2" s="1">
-        <v>264</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1418</v>
-      </c>
-      <c r="J2" s="1">
-        <v>720</v>
-      </c>
-      <c r="K2" s="1">
-        <v>645</v>
-      </c>
-      <c r="L2" s="1">
-        <v>1521</v>
-      </c>
-      <c r="M2" s="1">
-        <v>1284</v>
-      </c>
-      <c r="N2" s="1">
-        <v>583</v>
-      </c>
-      <c r="O2" s="1">
-        <v>54</v>
-      </c>
-      <c r="P2" s="1">
-        <v>396</v>
-      </c>
-      <c r="Q2" s="1">
-        <v>305</v>
-      </c>
-      <c r="R2" s="1">
-        <v>305</v>
-      </c>
-      <c r="S2" s="1">
-        <v>150</v>
-      </c>
-      <c r="T2" s="1">
-        <v>458</v>
-      </c>
-      <c r="U2" s="1">
-        <v>17137</v>
+      <c r="D2" s="5">
+        <v>1672</v>
+      </c>
+      <c r="E2" s="5">
+        <v>3403</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1958</v>
+      </c>
+      <c r="G2" s="5">
+        <v>205</v>
+      </c>
+      <c r="H2" s="5">
+        <v>310</v>
+      </c>
+      <c r="I2" s="5">
+        <v>1292</v>
+      </c>
+      <c r="J2" s="5">
+        <v>4292</v>
+      </c>
+      <c r="K2" s="5">
+        <v>532</v>
+      </c>
+      <c r="L2" s="5">
+        <v>1634</v>
+      </c>
+      <c r="M2" s="5">
+        <v>1518</v>
+      </c>
+      <c r="N2" s="5">
+        <v>578</v>
+      </c>
+      <c r="O2" s="5">
+        <v>75</v>
+      </c>
+      <c r="P2" s="5">
+        <v>827</v>
+      </c>
+      <c r="Q2" s="5">
+        <v>434</v>
+      </c>
+      <c r="R2" s="5">
+        <v>120</v>
+      </c>
+      <c r="S2" s="5">
+        <v>319</v>
+      </c>
+      <c r="T2" s="5">
+        <v>447</v>
+      </c>
+      <c r="U2" s="5">
+        <v>19616</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9549,59 +9566,59 @@
       <c r="C3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="1">
-        <v>57</v>
-      </c>
-      <c r="E3" s="1">
-        <v>42</v>
-      </c>
-      <c r="F3" s="1">
-        <v>13</v>
-      </c>
-      <c r="G3" s="1">
-        <v>13</v>
-      </c>
-      <c r="H3" s="1">
-        <v>44</v>
-      </c>
-      <c r="I3" s="1">
-        <v>19</v>
-      </c>
-      <c r="J3" s="1">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1">
-        <v>9</v>
-      </c>
-      <c r="L3" s="1">
-        <v>46</v>
-      </c>
-      <c r="M3" s="1">
-        <v>65</v>
-      </c>
-      <c r="N3" s="1">
-        <v>13</v>
-      </c>
-      <c r="O3" s="1">
-        <v>1</v>
-      </c>
-      <c r="P3" s="1">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="1">
-        <v>0</v>
-      </c>
-      <c r="R3" s="1">
-        <v>23</v>
-      </c>
-      <c r="S3" s="1">
-        <v>1</v>
-      </c>
-      <c r="T3" s="1">
-        <v>103</v>
-      </c>
-      <c r="U3" s="1">
-        <v>462</v>
+      <c r="D3" s="5">
+        <v>254</v>
+      </c>
+      <c r="E3" s="5">
+        <v>690</v>
+      </c>
+      <c r="F3" s="5">
+        <v>289</v>
+      </c>
+      <c r="G3" s="5">
+        <v>34</v>
+      </c>
+      <c r="H3" s="5">
+        <v>86</v>
+      </c>
+      <c r="I3" s="5">
+        <v>345</v>
+      </c>
+      <c r="J3" s="5">
+        <v>614</v>
+      </c>
+      <c r="K3" s="5">
+        <v>47</v>
+      </c>
+      <c r="L3" s="5">
+        <v>357</v>
+      </c>
+      <c r="M3" s="5">
+        <v>146</v>
+      </c>
+      <c r="N3" s="5">
+        <v>94</v>
+      </c>
+      <c r="O3" s="5">
+        <v>20</v>
+      </c>
+      <c r="P3" s="5">
+        <v>123</v>
+      </c>
+      <c r="Q3" s="5">
+        <v>131</v>
+      </c>
+      <c r="R3" s="5">
+        <v>22</v>
+      </c>
+      <c r="S3" s="5">
+        <v>40</v>
+      </c>
+      <c r="T3" s="5">
+        <v>153</v>
+      </c>
+      <c r="U3" s="5">
+        <v>3445</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -13450,19 +13467,231 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E760129D-04FB-3449-87D4-E344802252E2}">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U4" sqref="U4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1988</v>
+      </c>
+      <c r="E2" s="2">
+        <v>3488</v>
+      </c>
+      <c r="F2" s="2">
+        <v>537</v>
+      </c>
+      <c r="G2" s="2">
+        <v>415</v>
+      </c>
+      <c r="H2" s="2">
+        <v>352</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1248</v>
+      </c>
+      <c r="J2" s="2">
+        <v>3248</v>
+      </c>
+      <c r="K2" s="2">
+        <v>455</v>
+      </c>
+      <c r="L2" s="2">
+        <v>1605</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1475</v>
+      </c>
+      <c r="N2" s="2">
+        <v>551</v>
+      </c>
+      <c r="O2" s="2">
+        <v>84</v>
+      </c>
+      <c r="P2" s="1">
+        <v>989</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>506</v>
+      </c>
+      <c r="R2" s="1">
+        <v>158</v>
+      </c>
+      <c r="S2" s="1">
+        <v>372</v>
+      </c>
+      <c r="T2" s="1">
+        <v>558</v>
+      </c>
+      <c r="U2" s="1">
+        <v>18029</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="5">
+        <v>255</v>
+      </c>
+      <c r="E3" s="5">
+        <v>535</v>
+      </c>
+      <c r="F3" s="5">
+        <v>376</v>
+      </c>
+      <c r="G3" s="5">
+        <v>88</v>
+      </c>
+      <c r="H3" s="5">
+        <v>43</v>
+      </c>
+      <c r="I3" s="5">
+        <v>273</v>
+      </c>
+      <c r="J3" s="5">
+        <v>367</v>
+      </c>
+      <c r="K3" s="5">
+        <v>33</v>
+      </c>
+      <c r="L3" s="5">
+        <v>356</v>
+      </c>
+      <c r="M3" s="5">
+        <v>148</v>
+      </c>
+      <c r="N3" s="5">
+        <v>58</v>
+      </c>
+      <c r="O3" s="5">
+        <v>20</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>122</v>
+      </c>
+      <c r="R3" s="1">
+        <v>36</v>
+      </c>
+      <c r="S3" s="1">
+        <v>51</v>
+      </c>
+      <c r="T3" s="1">
+        <v>166</v>
+      </c>
+      <c r="U3" s="1">
+        <v>3089</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:U958"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="8.6640625" customWidth="1"/>
     <col min="2" max="2" width="11.1640625" customWidth="1"/>
-    <col min="4" max="4" width="4.6640625" customWidth="1"/>
+    <col min="4" max="4" width="5.83203125" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" customWidth="1"/>
     <col min="6" max="6" width="4.6640625" customWidth="1"/>
     <col min="7" max="8" width="3.6640625" customWidth="1"/>
@@ -17510,6 +17739,426 @@
     <row r="958" spans="2:3" ht="13" x14ac:dyDescent="0.15">
       <c r="B958" s="2"/>
       <c r="C958" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31543497-1A17-A742-8604-C3998B06888F}">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:U3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="2">
+        <v>1874</v>
+      </c>
+      <c r="E2" s="2">
+        <v>2935</v>
+      </c>
+      <c r="F2" s="2">
+        <v>667</v>
+      </c>
+      <c r="G2" s="2">
+        <v>475</v>
+      </c>
+      <c r="H2" s="2">
+        <v>399</v>
+      </c>
+      <c r="I2" s="2">
+        <v>1102</v>
+      </c>
+      <c r="J2" s="2">
+        <v>3294</v>
+      </c>
+      <c r="K2" s="2">
+        <v>349</v>
+      </c>
+      <c r="L2" s="2">
+        <v>2011</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1607</v>
+      </c>
+      <c r="N2" s="2">
+        <v>447</v>
+      </c>
+      <c r="O2" s="1">
+        <v>102</v>
+      </c>
+      <c r="P2" s="1">
+        <v>772</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>348</v>
+      </c>
+      <c r="R2" s="1">
+        <v>325</v>
+      </c>
+      <c r="S2" s="1">
+        <v>211</v>
+      </c>
+      <c r="T2" s="1">
+        <v>290</v>
+      </c>
+      <c r="U2" s="1">
+        <v>17208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="2">
+        <v>340</v>
+      </c>
+      <c r="E3" s="2">
+        <v>382</v>
+      </c>
+      <c r="F3" s="2">
+        <v>439</v>
+      </c>
+      <c r="G3" s="2">
+        <v>131</v>
+      </c>
+      <c r="H3" s="2">
+        <v>46</v>
+      </c>
+      <c r="I3" s="2">
+        <v>380</v>
+      </c>
+      <c r="J3" s="2">
+        <v>381</v>
+      </c>
+      <c r="K3" s="2">
+        <v>32</v>
+      </c>
+      <c r="L3" s="2">
+        <v>376</v>
+      </c>
+      <c r="M3" s="2">
+        <v>193</v>
+      </c>
+      <c r="N3" s="2">
+        <v>46</v>
+      </c>
+      <c r="O3" s="1">
+        <v>18</v>
+      </c>
+      <c r="P3" s="1">
+        <v>105</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>48</v>
+      </c>
+      <c r="R3" s="1">
+        <v>21</v>
+      </c>
+      <c r="S3" s="1">
+        <v>55</v>
+      </c>
+      <c r="T3" s="1">
+        <v>157</v>
+      </c>
+      <c r="U3" s="1">
+        <v>3150</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DA3FEEB-0CCC-BE45-89C4-D96576E47888}">
+  <dimension ref="A1:U3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:U3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A2" s="1">
+        <v>4</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1956</v>
+      </c>
+      <c r="E2" s="1">
+        <v>1963</v>
+      </c>
+      <c r="F2" s="1">
+        <v>776</v>
+      </c>
+      <c r="G2" s="1">
+        <v>66</v>
+      </c>
+      <c r="H2" s="1">
+        <v>460</v>
+      </c>
+      <c r="I2" s="1">
+        <v>896</v>
+      </c>
+      <c r="J2" s="1">
+        <v>1899</v>
+      </c>
+      <c r="K2" s="1">
+        <v>323</v>
+      </c>
+      <c r="L2" s="1">
+        <v>1339</v>
+      </c>
+      <c r="M2" s="1">
+        <v>1706</v>
+      </c>
+      <c r="N2" s="1">
+        <v>467</v>
+      </c>
+      <c r="O2" s="1">
+        <v>145</v>
+      </c>
+      <c r="P2" s="1">
+        <v>620</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>350</v>
+      </c>
+      <c r="R2" s="1">
+        <v>359</v>
+      </c>
+      <c r="S2" s="1">
+        <v>207</v>
+      </c>
+      <c r="T2" s="1">
+        <v>417</v>
+      </c>
+      <c r="U2" s="1">
+        <v>13949</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+      <c r="A3" s="1">
+        <v>4</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" s="1">
+        <v>267</v>
+      </c>
+      <c r="E3" s="1">
+        <v>271</v>
+      </c>
+      <c r="F3" s="1">
+        <v>271</v>
+      </c>
+      <c r="G3" s="1">
+        <v>10</v>
+      </c>
+      <c r="H3" s="1">
+        <v>11</v>
+      </c>
+      <c r="I3" s="1">
+        <v>189</v>
+      </c>
+      <c r="J3" s="1">
+        <v>400</v>
+      </c>
+      <c r="K3" s="1">
+        <v>25</v>
+      </c>
+      <c r="L3" s="1">
+        <v>300</v>
+      </c>
+      <c r="M3" s="1">
+        <v>194</v>
+      </c>
+      <c r="N3" s="1">
+        <v>85</v>
+      </c>
+      <c r="O3" s="1">
+        <v>18</v>
+      </c>
+      <c r="P3" s="1">
+        <v>60</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>104</v>
+      </c>
+      <c r="R3" s="1">
+        <v>41</v>
+      </c>
+      <c r="S3" s="1">
+        <v>34</v>
+      </c>
+      <c r="T3" s="1">
+        <v>234</v>
+      </c>
+      <c r="U3" s="1">
+        <v>2514</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
@@ -31506,7 +32155,7 @@
   </sheetPr>
   <dimension ref="A1:V999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="174" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
@@ -43785,7 +44434,7 @@
   <dimension ref="A1:W957"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+      <selection activeCell="U7" sqref="U7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -43796,7 +44445,8 @@
     <col min="4" max="4" width="4.6640625" customWidth="1"/>
     <col min="5" max="5" width="5.1640625" customWidth="1"/>
     <col min="6" max="7" width="3.6640625" customWidth="1"/>
-    <col min="8" max="12" width="4.6640625" customWidth="1"/>
+    <col min="8" max="11" width="4.6640625" customWidth="1"/>
+    <col min="12" max="12" width="7" customWidth="1"/>
     <col min="13" max="19" width="3.6640625" customWidth="1"/>
     <col min="20" max="20" width="4.5" customWidth="1"/>
     <col min="21" max="21" width="5.83203125" customWidth="1"/>
@@ -43877,59 +44527,59 @@
       <c r="C2" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="D2" s="1">
-        <v>2774</v>
-      </c>
-      <c r="E2" s="1">
-        <v>8870</v>
-      </c>
-      <c r="F2" s="1">
-        <v>2716</v>
-      </c>
-      <c r="G2" s="1">
-        <v>262</v>
-      </c>
-      <c r="H2" s="1">
-        <v>238</v>
-      </c>
-      <c r="I2" s="1">
-        <v>1223</v>
-      </c>
-      <c r="J2" s="1">
-        <v>970</v>
-      </c>
-      <c r="K2" s="1">
-        <v>669</v>
-      </c>
-      <c r="L2" s="1">
-        <v>2413</v>
-      </c>
-      <c r="M2" s="1">
-        <v>2264</v>
-      </c>
-      <c r="N2" s="1">
-        <v>718</v>
-      </c>
-      <c r="O2" s="1">
-        <v>101</v>
+      <c r="D2" s="5">
+        <v>1547</v>
+      </c>
+      <c r="E2" s="5">
+        <v>3515</v>
+      </c>
+      <c r="F2" s="5">
+        <v>1777</v>
+      </c>
+      <c r="G2" s="5">
+        <v>254</v>
+      </c>
+      <c r="H2" s="5">
+        <v>294</v>
+      </c>
+      <c r="I2" s="5">
+        <v>1130</v>
+      </c>
+      <c r="J2" s="5">
+        <v>2586</v>
+      </c>
+      <c r="K2" s="5">
+        <v>423</v>
+      </c>
+      <c r="L2" s="5">
+        <v>1991</v>
+      </c>
+      <c r="M2" s="5">
+        <v>1578</v>
+      </c>
+      <c r="N2" s="5">
+        <v>616</v>
+      </c>
+      <c r="O2" s="5">
+        <v>153</v>
       </c>
       <c r="P2" s="1">
-        <v>1194</v>
+        <v>1023</v>
       </c>
       <c r="Q2" s="1">
-        <v>480</v>
+        <v>460</v>
       </c>
       <c r="R2" s="1">
-        <v>422</v>
+        <v>237</v>
       </c>
       <c r="S2" s="1">
-        <v>186</v>
+        <v>317</v>
       </c>
       <c r="T2" s="1">
-        <v>765</v>
+        <v>739</v>
       </c>
       <c r="U2" s="1">
-        <v>26265</v>
+        <v>18640</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -43942,59 +44592,59 @@
       <c r="C3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="1">
-        <v>76</v>
-      </c>
-      <c r="E3" s="1">
+      <c r="D3" s="5">
+        <v>278</v>
+      </c>
+      <c r="E3" s="5">
+        <v>647</v>
+      </c>
+      <c r="F3" s="5">
+        <v>252</v>
+      </c>
+      <c r="G3" s="5">
+        <v>60</v>
+      </c>
+      <c r="H3" s="5">
+        <v>61</v>
+      </c>
+      <c r="I3" s="5">
+        <v>255</v>
+      </c>
+      <c r="J3" s="5">
+        <v>921</v>
+      </c>
+      <c r="K3" s="5">
+        <v>112</v>
+      </c>
+      <c r="L3" s="5">
+        <v>391</v>
+      </c>
+      <c r="M3" s="5">
+        <v>360</v>
+      </c>
+      <c r="N3" s="5">
+        <v>81</v>
+      </c>
+      <c r="O3" s="5">
         <v>22</v>
       </c>
-      <c r="F3" s="1">
-        <v>258</v>
-      </c>
-      <c r="G3" s="1">
-        <v>17</v>
-      </c>
-      <c r="H3" s="1">
-        <v>40</v>
-      </c>
-      <c r="I3" s="1">
-        <v>6</v>
-      </c>
-      <c r="J3" s="1">
-        <v>8</v>
-      </c>
-      <c r="K3" s="1">
-        <v>39</v>
-      </c>
-      <c r="L3" s="1">
-        <v>63</v>
-      </c>
-      <c r="M3" s="1">
-        <v>164</v>
-      </c>
-      <c r="N3" s="1">
-        <v>16</v>
-      </c>
-      <c r="O3" s="1">
-        <v>0</v>
-      </c>
       <c r="P3" s="1">
-        <v>2</v>
+        <v>144</v>
       </c>
       <c r="Q3" s="1">
-        <v>0</v>
+        <v>81</v>
       </c>
       <c r="R3" s="1">
-        <v>23</v>
+        <v>48</v>
       </c>
       <c r="S3" s="1">
-        <v>1</v>
+        <v>59</v>
       </c>
       <c r="T3" s="1">
-        <v>164</v>
+        <v>178</v>
       </c>
       <c r="U3" s="1">
-        <v>899</v>
+        <v>3950</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -47840,8 +48490,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AE40049-9301-4942-A8D6-02C133D7751D}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S1" sqref="S1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -48056,7 +48706,9 @@
   </sheetPr>
   <dimension ref="A1:U1001"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>

</xml_diff>